<commit_message>
Localization of new checks in Korean.
</commit_message>
<xml_diff>
--- a/Config/KO/Checklist.xlsx
+++ b/Config/KO/Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus Cruz\Documents\GitHub\Workflow-Inspector\Config\KO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202387C-CAC6-416B-8DEA-1BD326D3498D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916E0B5C-1CDC-4641-BD27-CDCE1D5AF7A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,45 +421,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Undocumented Parallel activity</t>
-  </si>
-  <si>
     <t>Checks\Standard\UndocumentedParallelActivity.xaml</t>
   </si>
   <si>
-    <t>Using the Parallel activity can make the workflow harder to understand and might lead to unexpected results when combined with UI interactions. If it is necessary to use the Parallel activity, include an annotation to explain the situation.
-For more about the Parallel activity, please refer to https://docs.microsoft.com/en-us/dotnet/api/system.activities.statements.parallel?view=netframework-4.8</t>
-  </si>
-  <si>
-    <t>Verify whether the Parallel activity is really necessary and, if it is, include an annotation explaning why it is being used.</t>
-  </si>
-  <si>
-    <t>Hardcoded password</t>
-  </si>
-  <si>
     <t>Checks\Standard\HardcodedPassword.xaml</t>
   </si>
   <si>
-    <t>Passwords that are hardcoded into workflows can be a serious security threat since they can be easily recovered by unauthorized parties. For more about protecting sensitive data, please refer to https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
-  </si>
-  <si>
-    <t>Passwords should be stored in secure locations, like Orchestrator or Windows Credential Manager.</t>
-  </si>
-  <si>
-    <t>Undocumented Image-based activities</t>
-  </si>
-  <si>
     <t>Checks\Standard\UndocumentedImageBasedActivities.xaml</t>
-  </si>
-  <si>
-    <t>The use of image-based activities (e.g., Click Image and Wait Image Vanish) is not usually recommended, because they are sensitive to screen resolutions and image quality.
-In cases they must be used, it is a good practice to include an annotation to the activity to explain the situation.</t>
-  </si>
-  <si>
-    <t>Confirm whether image-based activities are really necessary and, if they are, add an annotation to explain the situation.</t>
-  </si>
-  <si>
-    <t>Workflow naming convention</t>
   </si>
   <si>
     <t>Checks\Custom\WorkflowFileNamingConvention.xaml</t>
@@ -468,16 +436,6 @@
     <t>{ 
 "NamingPattern" : "^[A-Z0-9]{7}_[0-9]{3}_.*$"
 }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workflows in a project should be named according to the project's naming conventions.  This check receives a regular expression that dictates the naming convention for workflow files. </t>
-  </si>
-  <si>
-    <t>Change the name of the file to match the project's naming conventions.</t>
-  </si>
-  <si>
-    <t>Mandatory files in project</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Checks\Custom\MandatoryFilesInProject.xaml</t>
@@ -490,11 +448,592 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>The project should contain mandatory files specified by the COE or project leader. This check receives a list of files that should be in the project folder.</t>
+    <t>문서화되지 않은 병렬 액티비티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>병렬 액티비티 사용은 워크플로우를 이해하기 어렵게 만들며, UI 상호작용시 기대하지 않은 결과를 도출할수 있습니다. 병렬 액티비티의 사용이 필요하다면 상황을 설명을 하는 주석을 추가하주세요. 병령 액티비티의 자세한 내용은 아래 링크를 참고 하세요. https://docs.microsoft.com/en-us/dotnet/api/system.activities.statements.parallel?view=netframework-4.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>병렬 액티비티가 정말로 필요한지 확인하세요. 만약 필요하다면 필요한 이유를 주석으로 추가하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하드코드된 비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호가 하드코드된 상태로 워크플로우에 존재하는 경우 심각한 보안 위협이 됩니다. 하드코드된 비빌번호는 누구나 쉽게 읽을수 있습니다. 민감한 데이터 보호하기 관련해서는 아래 링크를 참고하세요. https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">비밀번호는 오케스트레이터나 윈도우 비밀번호 관리자 같은 안전한 저장소에 저장되어야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문서화되지 않은 이미지 기반 액티비티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Click Image 와 Wait Image Vanish같은 이미지 기반 액티비티의 사용은 일반적으로 권고되지 않습니다. 이러한 액티비티는 스크린 해상도와 이미지 품질에 민감하기 때문입니다. 이미지 기반 액티비티가 반드시 사용되어야 하는 경우 이러한 상황을 설명하는 주석을 추가하는 것이 좋습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 기반 액티비티가 정말로 필요한지 확인하세요. 만약 그렇다면 상황을 설명하는 주석을 추가하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워크플로우 명명 규칙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">워크플로우 파일 이름은 프로젝트 명명 규칙에 맞아야 합니다. 이 점검은 정규식 표현으로 워크플로우 파일 이름 규칙을 기술합니다.  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 명명 규칙에 맞게 워크플로우 파일 이름을 변경하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>필수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Include the mandatory files in the project folder.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> COE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>혹은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>리더가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지정한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>필수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>포함해야</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>합니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>점검은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>폴더에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>반드시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>존재해야</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>필수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>목록을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검사합니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>폴더에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>필수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>추가하세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -502,7 +1041,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -577,6 +1116,26 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -639,7 +1198,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -689,6 +1248,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1406,25 +1968,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="132">
+    <row r="19" spans="1:7" ht="115.5">
       <c r="A19" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="82.5">
@@ -1432,20 +1994,20 @@
         <v>0</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="82.5">
@@ -1453,20 +2015,20 @@
         <v>0</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="99">
@@ -1474,22 +2036,22 @@
         <v>0</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="49.5">
@@ -1566,9 +2128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D4DFEF-ABB7-4679-8B2C-373516D40D24}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5"/>
   <cols>
@@ -1650,22 +2210,22 @@
       <c r="A4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>128</v>
+      <c r="B4" s="18" t="s">
+        <v>130</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="18" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include Korean translation of new checks
</commit_message>
<xml_diff>
--- a/Config/KO/Checklist.xlsx
+++ b/Config/KO/Checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\Workflow-Inspector\Config\KO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801605A6-FE03-447A-B8BE-C50BF7327EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5AF5D4-46DF-4E1E-B1BB-D60EFC45879B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1136,43 +1136,13 @@
     <t>로그 브라우저 URL</t>
   </si>
   <si>
-    <t>Unadjusted For Each</t>
-  </si>
-  <si>
     <t>Checks\Standard\UnadjustedForEach.xaml</t>
   </si>
   <si>
-    <t>To further improve the readability of the workflow, it is recommended to change the name and type of the "item" loop variable in the For Each activity according to the data being processed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modify the type and the name of the "item" loop variable in the For Each activity to match the data being processed. </t>
-  </si>
-  <si>
-    <t>Missing project entry point workflow</t>
-  </si>
-  <si>
     <t>Checks\Standard\MissingProjectEntryPointWorkflow.xaml</t>
   </si>
   <si>
-    <t>The project.json configuration file defines a workflow (usually Main.xaml) to act as the entry point for the project and this workflow should be included in the project.</t>
-  </si>
-  <si>
-    <t>Make sure the project contains the entry point workflow as defined in project.json.</t>
-  </si>
-  <si>
-    <t>Unallowed application</t>
-  </si>
-  <si>
     <t>Checks\Custom\UnallowedApplication.xaml</t>
-  </si>
-  <si>
-    <t>Workflows should interact only with applications allowed by the Centre of Excellence (CoE). If an application is present in the blacklist or is not present in the whitelist of activities, it should not be used by the robot. The whitelist and the blacklist are passed as arguments to this check and contain names of applications' executable files. Each name must be specified as the application's executable file name (for example, "notepad.exe" instead of "Notepad").</t>
-  </si>
-  <si>
-    <t>Remove interactions with unallowed applications from the workflow or request the addition of the application to the whitelist (or its removal from the blacklist).</t>
-  </si>
-  <si>
-    <t>Activity naming convention</t>
   </si>
   <si>
     <t>Checks\Custom\ActivityNamingConvention.xaml</t>
@@ -1183,23 +1153,7 @@
 }</t>
   </si>
   <si>
-    <t>Activities in a project should follow a specified naming convention, since it makes it easier to understand the project and maintain it. This check receives a regular expression that dictates the naming convention for activities.</t>
-  </si>
-  <si>
-    <t>Change the name of the activity to match the project's naming conventions.</t>
-  </si>
-  <si>
-    <t>No User Interaction</t>
-  </si>
-  <si>
     <t>Checks\Custom\NoUserInteraction.xaml</t>
-  </si>
-  <si>
-    <t>Unattended robots are expected to work in an unattended terminal environment, so do not display message dialogs or input dialogs to users. This prevents the Unattended robot from stopping by requesting user interaction.
-This check checks that no activities that require user interaction are used.</t>
-  </si>
-  <si>
-    <t>If the process is to be run on Unattended robots, remove activities that expect user interaction.</t>
   </si>
   <si>
     <t>{ 
@@ -1218,19 +1172,7 @@
 } </t>
   </si>
   <si>
-    <t>Unsuitable exception type</t>
-  </si>
-  <si>
     <t>Checks\Custom\UnsuitableExceptionType.xaml</t>
-  </si>
-  <si>
-    <t>When throwing exceptions, it is recommended to properly distinguish between application-originated and business-originated exceptions. The type of the exception to be thrown or caught should be as specific as possible, and Exception and ApplicationException should be avoided.</t>
-  </si>
-  <si>
-    <t>Use specific exception types and avoid using generic types such as Exception and ApplicationException.</t>
-  </si>
-  <si>
-    <t>ReadOnly property of constant</t>
   </si>
   <si>
     <t>Checks\Custom\ReadOnlyPropertyOfConstant.xaml</t>
@@ -1241,30 +1183,583 @@
 }</t>
   </si>
   <si>
-    <t>Constant is a variable that does not change the value set by the default value. 
-It must follow a specific naming convention so that it can be distinguished from other variables. In addition, ReadOnly must be specified in the variable's Modifiers property.</t>
-  </si>
-  <si>
-    <t>Variables that do not have their values modified should follow the naming convention of constants and have ReadOnly checked in their Modifiers property.</t>
-  </si>
-  <si>
-    <t>Directly send Outlook mail</t>
-  </si>
-  <si>
     <t>Checks\Custom\DirectlySendOutlookMail.xaml</t>
   </si>
   <si>
-    <t>Check the IsDraft property of Send Outlook Mail Message activities, as specified by the CoE's security policies.</t>
-  </si>
-  <si>
-    <t>According to the CoE (Centre of Excellence)'s security policies, robots should not be allowed to directly send emails. Instead, emails created by robots should be saved as drafts and then reviewed by humans before sending.</t>
+    <t xml:space="preserve">Check the IsDraft property of Send Outlook Mail Message activities, as specified by the CoE's security policies. CoE보안 정책에 준해서 아웃룩 메일 보내기 액티비티에서 IsDraft 속성을 선택하세요. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">누락된 시작 워크플로우 파일 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(project.json)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기본값으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Main.xaml </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>워크플로우</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지정합니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>워크플로우</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>반드시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>포함되어야</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>합니다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>워크플로우</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>파일이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지정되어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>확인하세요</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아웃룩 메일 직접 전송</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoE의 보안 정책에 따라 로봇은 이메일을 직접 보내지 못하도록 구성되어야 합니다. 이메일은 로봇에 의해서 초안으로 저장되고 보내기 전에 담당자(사람)에 의한 검토되어야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">변수의 값이 변경되지 않는다면 변수 속성에서 읽기 전용을 체크하세요. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception 혹은 ApplicationException 같은 타입을 사용하지 말고 구체적인 예외 타입을 사용하세요. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예외를 발생시키는 경우 애플리케이션 관련 예외인지 비지니스 관련 예외인지 구분하는 것을 권고합니다. 가능한 예외는 구체적으로 지정하기를 권고합니다. 예를 들어 Exception 혹은 ApplicationException 같은 예외 타입은 사용하지 마시고 구체적인 예외 타입을 사용하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>만약 프로세스가 무인로봇에서 실행된다면 사용자 상호동작을 기대하는 액티비티를 제거하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트의 명명 규칙에 맞게 액티비티 이름을 변경하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">프로젝트에 포함된 액티비티들은 정해진 명명 규칙을 따라야 합니다. 이 규직은 프로젝트를 이해하기 쉽게하고 유지보수를 수월하게 해줍니다. 이 점검은 정규식 표현으로 액티비티 이름 규칙을 기술합니다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상수 변수에 대한 읽기 전용 속성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상수 변수는 초기 값으로 설정된 이후 변경되지 않습니다. 상수 변수는 지정된 명명 규칙을 따라야 하며 다른 변수와는 구분되어야 합니다. 변수 속성에서 읽기 전용이 체크되어야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 상호작용 없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부적절한 예외 타입</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무인로봇은 무인 환경에서 수행됩니다. 따라서 사용자에게 안내 메세지 혹은 입력 다이얼로그를 보여주지 마세요. 이 점검은 사용자 상호동작 액티비티로 인해 발생할 수 있는 멈춤 현상을 없앨 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>액티비티 명명 규칙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">허용되지 않는 애플리케이션 </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">워크플로우는 CoE에서 허용한 애플리케이션들과 상호작용해야 합니다. 만약 애플리케이션이 거부목록에 포함되어 있거나 혹은 허용목록에 포함되어 있지 않다면 이 애플리케이션은 로봇에 의해 사용되지 않아야 합니다. 거부목록과 허용목록은 이 점검의 인수로 전달되며 애플리케이션의 실행화일이 각 목록에 포함되어 있습니다. 각각의 이름은 애플리케이션의 실행파일 이름입니다. (예, Notepad의 경우 Notepad가 아니라 notepad.exe 이여야 합니다) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>허용되지 않은 애플리케이션과의 상호작용을 제거하거나 해당 애플리케이션을 허용목록에 추가되거나, 거부목록에서 제거되도록 CoE에 요청하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>조정되지 않은 For Each 액티비티</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">워크플로우의 가독성을 향상시키기 위해 For Each 액티비티의 반복문에서 사용되는 item 변수의 이름을 처리하는 데이터와 관련된 이름으로 변경하는 것을 권고합니다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Each 반복문에서 사용되는 item 변수의 타입과 이름을 처리하는 데이터와 관련된 타입과 이름으로 변경하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1373,6 +1868,20 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1435,7 +1944,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1512,6 +2021,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1827,15 +2339,15 @@
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="14.1796875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="15" customWidth="1"/>
     <col min="3" max="3" width="40.1796875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" style="15" customWidth="1"/>
     <col min="6" max="6" width="64.1796875" style="15" customWidth="1"/>
     <col min="7" max="7" width="33.453125" style="15" customWidth="1"/>
     <col min="8" max="8" width="8.81640625" style="14"/>
-    <col min="9" max="9" width="41.54296875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="51.54296875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="41.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="51.453125" style="14" customWidth="1"/>
     <col min="11" max="16384" width="8.81640625" style="14"/>
   </cols>
   <sheetData>
@@ -1957,7 +2469,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>3</v>
@@ -1980,7 +2492,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>3</v>
@@ -2145,7 +2657,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="85">
+    <row r="15" spans="1:10" ht="68">
       <c r="A15" s="13" t="s">
         <v>71</v>
       </c>
@@ -2189,7 +2701,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="102">
+    <row r="17" spans="1:7" ht="85">
       <c r="A17" s="13" t="s">
         <v>71</v>
       </c>
@@ -2294,7 +2806,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="51">
+    <row r="22" spans="1:7" ht="35">
       <c r="A22" s="13" t="s">
         <v>0</v>
       </c>
@@ -2362,20 +2874,20 @@
         <v>0</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="187">
@@ -2406,22 +2918,22 @@
         <v>133</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="85">
@@ -2473,43 +2985,43 @@
         <v>128</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="102">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="68">
       <c r="A31" s="19" t="s">
         <v>128</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="85">
@@ -2517,20 +3029,20 @@
         <v>128</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="85">
@@ -2538,43 +3050,43 @@
         <v>128</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="68">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="119">
       <c r="A34" s="19" t="s">
         <v>128</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2593,18 +3105,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D4DFEF-ABB7-4679-8B2C-373516D40D24}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="31.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="31.453125" style="3" customWidth="1"/>
     <col min="6" max="6" width="55.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="44.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="44.453125" style="3" customWidth="1"/>
     <col min="8" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
@@ -2673,25 +3185,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" ht="43.5">
+    <row r="4" spans="1:7" s="26" customFormat="1" ht="51">
       <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>150</v>
+      <c r="F4" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="188.5">

</xml_diff>